<commit_message>
Cleaned up repo and added combine reporting
</commit_message>
<xml_diff>
--- a/CDE_ID_detective_revamp/ReRun/Data_Dictionary_Tracker_as_of_2025-07-08.xlsx
+++ b/CDE_ID_detective_revamp/ReRun/Data_Dictionary_Tracker_as_of_2025-07-08.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmaefos\Code Stuffs\CDE_detective\CDE_ID_detective_revamp\ReRun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D7CF2A-E448-4FFD-AC33-2D5F0526340A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E5B437-00CE-4295-BCFE-A2658E5CBFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38790" yWindow="7110" windowWidth="11400" windowHeight="18480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data dictionary track" sheetId="1" r:id="rId1"/>
@@ -1575,7 +1575,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1741,6 +1741,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2163,7 +2169,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2452,6 +2458,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="34" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="34" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2817,10 +2836,10 @@
   <dimension ref="A1:AN58"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="23" ySplit="2" topLeftCell="Z3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="23" ySplit="2" topLeftCell="AA3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AA30" sqref="AA30"/>
+      <selection pane="bottomRight" activeCell="AA29" sqref="AA29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -3065,7 +3084,7 @@
       <c r="Z3" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AA3" s="106" t="s">
         <v>410</v>
       </c>
       <c r="AB3" s="6"/>
@@ -3183,7 +3202,7 @@
       <c r="Z4" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="AA4" s="6" t="s">
+      <c r="AA4" s="106" t="s">
         <v>414</v>
       </c>
       <c r="AB4" s="6"/>
@@ -3303,7 +3322,7 @@
       <c r="Z5" s="54" t="s">
         <v>354</v>
       </c>
-      <c r="AA5" s="31" t="s">
+      <c r="AA5" s="107" t="s">
         <v>415</v>
       </c>
       <c r="AB5" s="31"/>
@@ -3413,7 +3432,7 @@
       <c r="Z6" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="AA6" s="6" t="s">
+      <c r="AA6" s="106" t="s">
         <v>416</v>
       </c>
       <c r="AB6" s="6"/>
@@ -3533,7 +3552,7 @@
       <c r="Z7" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="AA7" s="6" t="s">
+      <c r="AA7" s="106" t="s">
         <v>417</v>
       </c>
       <c r="AB7" s="6"/>
@@ -3645,7 +3664,7 @@
       <c r="Z8" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="AA8" s="6" t="s">
+      <c r="AA8" s="106" t="s">
         <v>418</v>
       </c>
       <c r="AB8" s="6"/>
@@ -3757,7 +3776,7 @@
       <c r="Z9" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="AA9" s="6" t="s">
+      <c r="AA9" s="106" t="s">
         <v>424</v>
       </c>
       <c r="AB9" s="6"/>
@@ -3871,7 +3890,7 @@
       <c r="Z10" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="AA10" s="6" t="s">
+      <c r="AA10" s="106" t="s">
         <v>425</v>
       </c>
       <c r="AB10" s="6"/>
@@ -3983,7 +4002,7 @@
       <c r="Z11" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="AA11" s="6" t="s">
+      <c r="AA11" s="106" t="s">
         <v>419</v>
       </c>
       <c r="AB11" s="6"/>
@@ -4101,7 +4120,7 @@
       <c r="Z12" s="54" t="s">
         <v>358</v>
       </c>
-      <c r="AA12" s="6" t="s">
+      <c r="AA12" s="106" t="s">
         <v>420</v>
       </c>
       <c r="AB12" s="31"/>
@@ -4219,7 +4238,7 @@
       <c r="Z13" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="AA13" s="6" t="s">
+      <c r="AA13" s="106" t="s">
         <v>421</v>
       </c>
       <c r="AB13" s="6"/>
@@ -4333,7 +4352,7 @@
       <c r="Z14" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="AA14" s="6" t="s">
+      <c r="AA14" s="106" t="s">
         <v>422</v>
       </c>
       <c r="AB14" s="6"/>
@@ -4449,7 +4468,7 @@
       <c r="Z15" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="AA15" s="6" t="s">
+      <c r="AA15" s="106" t="s">
         <v>426</v>
       </c>
       <c r="AB15" s="6"/>
@@ -4567,7 +4586,7 @@
       <c r="Z16" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="AA16" s="6" t="s">
+      <c r="AA16" s="106" t="s">
         <v>423</v>
       </c>
       <c r="AB16" s="6"/>
@@ -4683,7 +4702,7 @@
       <c r="Z17" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AA17" s="108" t="s">
         <v>427</v>
       </c>
       <c r="AB17" s="6"/>
@@ -4795,7 +4814,7 @@
       <c r="Z18" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="AA18" s="6" t="s">
+      <c r="AA18" s="106" t="s">
         <v>428</v>
       </c>
       <c r="AB18" s="6"/>
@@ -4909,7 +4928,7 @@
       <c r="Z19" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="AA19" s="6" t="s">
+      <c r="AA19" s="106" t="s">
         <v>429</v>
       </c>
       <c r="AB19" s="6"/>
@@ -5021,7 +5040,7 @@
       <c r="Z20" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="AA20" s="6" t="s">
+      <c r="AA20" s="106" t="s">
         <v>430</v>
       </c>
       <c r="AB20" s="6"/>
@@ -5141,7 +5160,7 @@
       <c r="Z21" s="54" t="s">
         <v>346</v>
       </c>
-      <c r="AA21" s="31" t="s">
+      <c r="AA21" s="107" t="s">
         <v>431</v>
       </c>
       <c r="AB21" s="31"/>
@@ -5259,7 +5278,7 @@
       <c r="Z22" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="AA22" s="6" t="s">
+      <c r="AA22" s="106" t="s">
         <v>432</v>
       </c>
       <c r="AB22" s="6"/>
@@ -5371,7 +5390,7 @@
       <c r="Z23" s="101" t="s">
         <v>404</v>
       </c>
-      <c r="AA23" s="6" t="s">
+      <c r="AA23" s="106" t="s">
         <v>433</v>
       </c>
       <c r="AB23" s="6"/>
@@ -5483,7 +5502,7 @@
       <c r="Z24" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="AA24" s="6" t="s">
+      <c r="AA24" s="106" t="s">
         <v>434</v>
       </c>
       <c r="AB24" s="6"/>
@@ -5601,7 +5620,7 @@
       <c r="Z25" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="AA25" s="6" t="s">
+      <c r="AA25" s="106" t="s">
         <v>435</v>
       </c>
       <c r="AB25" s="6"/>
@@ -5721,7 +5740,7 @@
       <c r="Z26" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="AA26" s="6" t="s">
+      <c r="AA26" s="106" t="s">
         <v>436</v>
       </c>
       <c r="AB26" s="6"/>
@@ -7927,7 +7946,7 @@
       <c r="Y47" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="Z47" s="66" t="s">
+      <c r="Z47" s="104" t="s">
         <v>362</v>
       </c>
       <c r="AA47" s="66" t="s">
@@ -8045,7 +8064,7 @@
       <c r="Y48" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="Z48" s="102" t="s">
+      <c r="Z48" s="105" t="s">
         <v>401</v>
       </c>
       <c r="AA48" s="103" t="s">
@@ -8163,7 +8182,7 @@
       <c r="Y49" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="Z49" s="66" t="s">
+      <c r="Z49" s="104" t="s">
         <v>343</v>
       </c>
       <c r="AA49" s="66" t="s">
@@ -8281,7 +8300,7 @@
       <c r="Y50" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="Z50" s="102" t="s">
+      <c r="Z50" s="105" t="s">
         <v>364</v>
       </c>
       <c r="AA50" s="102" t="s">

</xml_diff>